<commit_message>
Added monthly trends to RSTs
</commit_message>
<xml_diff>
--- a/python/Statistics/Results/RST_classification_ERA_1979-2016.xlsx
+++ b/python/Statistics/Results/RST_classification_ERA_1979-2016.xlsx
@@ -1,21 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hatzv\Documents\Geography\RSTs\python\Statistics\Results\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14246" uniqueCount="16">
   <si>
     <t>No RST</t>
   </si>
@@ -28,30 +32,80 @@
   <si>
     <t>West</t>
   </si>
+  <si>
+    <t>Jan</t>
+  </si>
+  <si>
+    <t>Feb</t>
+  </si>
+  <si>
+    <t>Mar</t>
+  </si>
+  <si>
+    <t>Apr</t>
+  </si>
+  <si>
+    <t>May</t>
+  </si>
+  <si>
+    <t>Jun</t>
+  </si>
+  <si>
+    <t>Jul</t>
+  </si>
+  <si>
+    <t>Aug</t>
+  </si>
+  <si>
+    <t>Sep</t>
+  </si>
+  <si>
+    <t>Oct</t>
+  </si>
+  <si>
+    <t>Nov</t>
+  </si>
+  <si>
+    <t>Dec</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="10"/>
+      <color indexed="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color indexed="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -59,17 +113,47 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+  <cellXfs count="5">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -357,20 +441,136 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="B2:AM367"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AM367"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:39">
+    <row r="1" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="2">
+        <v>1979</v>
+      </c>
+      <c r="C1" s="2">
+        <v>1980</v>
+      </c>
+      <c r="D1" s="2">
+        <v>1981</v>
+      </c>
+      <c r="E1" s="2">
+        <v>1982</v>
+      </c>
+      <c r="F1" s="2">
+        <v>1983</v>
+      </c>
+      <c r="G1" s="2">
+        <v>1984</v>
+      </c>
+      <c r="H1" s="2">
+        <v>1985</v>
+      </c>
+      <c r="I1" s="2">
+        <v>1986</v>
+      </c>
+      <c r="J1" s="2">
+        <v>1987</v>
+      </c>
+      <c r="K1" s="2">
+        <v>1988</v>
+      </c>
+      <c r="L1" s="2">
+        <v>1989</v>
+      </c>
+      <c r="M1" s="2">
+        <v>1990</v>
+      </c>
+      <c r="N1" s="2">
+        <v>1991</v>
+      </c>
+      <c r="O1" s="2">
+        <v>1992</v>
+      </c>
+      <c r="P1" s="2">
+        <v>1993</v>
+      </c>
+      <c r="Q1" s="2">
+        <v>1994</v>
+      </c>
+      <c r="R1" s="2">
+        <v>1995</v>
+      </c>
+      <c r="S1" s="2">
+        <v>1996</v>
+      </c>
+      <c r="T1" s="2">
+        <v>1997</v>
+      </c>
+      <c r="U1" s="2">
+        <v>1998</v>
+      </c>
+      <c r="V1" s="2">
+        <v>1999</v>
+      </c>
+      <c r="W1" s="2">
+        <v>2000</v>
+      </c>
+      <c r="X1" s="2">
+        <v>2001</v>
+      </c>
+      <c r="Y1" s="2">
+        <v>2002</v>
+      </c>
+      <c r="Z1" s="2">
+        <v>2003</v>
+      </c>
+      <c r="AA1" s="2">
+        <v>2004</v>
+      </c>
+      <c r="AB1" s="2">
+        <v>2005</v>
+      </c>
+      <c r="AC1" s="2">
+        <v>2006</v>
+      </c>
+      <c r="AD1" s="2">
+        <v>2007</v>
+      </c>
+      <c r="AE1" s="2">
+        <v>2008</v>
+      </c>
+      <c r="AF1" s="2">
+        <v>2009</v>
+      </c>
+      <c r="AG1" s="2">
+        <v>2010</v>
+      </c>
+      <c r="AH1" s="2">
+        <v>2011</v>
+      </c>
+      <c r="AI1" s="2">
+        <v>2012</v>
+      </c>
+      <c r="AJ1" s="2">
+        <v>2013</v>
+      </c>
+      <c r="AK1" s="2">
+        <v>2014</v>
+      </c>
+      <c r="AL1" s="2">
+        <v>2015</v>
+      </c>
+      <c r="AM1" s="3">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="2" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -486,7 +686,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:39">
+    <row r="3" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -602,7 +805,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:39">
+    <row r="4" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="B4" t="s">
         <v>0</v>
       </c>
@@ -718,7 +924,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:39">
+    <row r="5" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="B5" t="s">
         <v>0</v>
       </c>
@@ -834,7 +1043,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:39">
+    <row r="6" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="B6" t="s">
         <v>0</v>
       </c>
@@ -950,7 +1162,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:39">
+    <row r="7" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="B7" t="s">
         <v>0</v>
       </c>
@@ -1066,7 +1281,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:39">
+    <row r="8" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="B8" t="s">
         <v>0</v>
       </c>
@@ -1182,7 +1400,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:39">
+    <row r="9" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="B9" t="s">
         <v>0</v>
       </c>
@@ -1298,7 +1519,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:39">
+    <row r="10" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="B10" t="s">
         <v>0</v>
       </c>
@@ -1414,7 +1638,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:39">
+    <row r="11" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="B11" t="s">
         <v>0</v>
       </c>
@@ -1530,7 +1757,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:39">
+    <row r="12" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="B12" t="s">
         <v>0</v>
       </c>
@@ -1646,7 +1876,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:39">
+    <row r="13" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="B13" t="s">
         <v>2</v>
       </c>
@@ -1762,7 +1995,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:39">
+    <row r="14" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="B14" t="s">
         <v>2</v>
       </c>
@@ -1878,7 +2114,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:39">
+    <row r="15" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="B15" t="s">
         <v>0</v>
       </c>
@@ -1994,7 +2233,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:39">
+    <row r="16" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="B16" t="s">
         <v>2</v>
       </c>
@@ -2110,7 +2352,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:39">
+    <row r="17" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="B17" t="s">
         <v>0</v>
       </c>
@@ -2226,7 +2471,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:39">
+    <row r="18" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="B18" t="s">
         <v>2</v>
       </c>
@@ -2342,7 +2590,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:39">
+    <row r="19" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="B19" t="s">
         <v>2</v>
       </c>
@@ -2458,7 +2709,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:39">
+    <row r="20" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="B20" t="s">
         <v>0</v>
       </c>
@@ -2574,7 +2828,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:39">
+    <row r="21" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="B21" t="s">
         <v>0</v>
       </c>
@@ -2690,7 +2947,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:39">
+    <row r="22" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="B22" t="s">
         <v>0</v>
       </c>
@@ -2806,7 +3066,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:39">
+    <row r="23" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="B23" t="s">
         <v>0</v>
       </c>
@@ -2922,7 +3185,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:39">
+    <row r="24" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="B24" t="s">
         <v>0</v>
       </c>
@@ -3038,7 +3304,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:39">
+    <row r="25" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="B25" t="s">
         <v>0</v>
       </c>
@@ -3154,7 +3423,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:39">
+    <row r="26" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="B26" t="s">
         <v>0</v>
       </c>
@@ -3270,7 +3542,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:39">
+    <row r="27" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="B27" t="s">
         <v>1</v>
       </c>
@@ -3386,7 +3661,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:39">
+    <row r="28" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="B28" t="s">
         <v>0</v>
       </c>
@@ -3502,7 +3780,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:39">
+    <row r="29" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="B29" t="s">
         <v>2</v>
       </c>
@@ -3618,7 +3899,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:39">
+    <row r="30" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="B30" t="s">
         <v>0</v>
       </c>
@@ -3734,7 +4018,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:39">
+    <row r="31" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="B31" t="s">
         <v>1</v>
       </c>
@@ -3850,7 +4137,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:39">
+    <row r="32" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="4" t="s">
+        <v>4</v>
+      </c>
       <c r="B32" t="s">
         <v>0</v>
       </c>
@@ -3966,7 +4256,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:39">
+    <row r="33" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="B33" t="s">
         <v>3</v>
       </c>
@@ -4082,7 +4375,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:39">
+    <row r="34" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="B34" t="s">
         <v>0</v>
       </c>
@@ -4198,7 +4494,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:39">
+    <row r="35" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="B35" t="s">
         <v>0</v>
       </c>
@@ -4314,7 +4613,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:39">
+    <row r="36" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="B36" t="s">
         <v>0</v>
       </c>
@@ -4430,7 +4732,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:39">
+    <row r="37" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="B37" t="s">
         <v>0</v>
       </c>
@@ -4546,7 +4851,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:39">
+    <row r="38" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="B38" t="s">
         <v>0</v>
       </c>
@@ -4662,7 +4970,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:39">
+    <row r="39" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="B39" t="s">
         <v>0</v>
       </c>
@@ -4778,7 +5089,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:39">
+    <row r="40" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="B40" t="s">
         <v>0</v>
       </c>
@@ -4894,7 +5208,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:39">
+    <row r="41" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="B41" t="s">
         <v>0</v>
       </c>
@@ -5010,7 +5327,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:39">
+    <row r="42" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="B42" t="s">
         <v>0</v>
       </c>
@@ -5126,7 +5446,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:39">
+    <row r="43" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="B43" t="s">
         <v>0</v>
       </c>
@@ -5242,7 +5565,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:39">
+    <row r="44" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="B44" t="s">
         <v>0</v>
       </c>
@@ -5358,7 +5684,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:39">
+    <row r="45" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="B45" t="s">
         <v>1</v>
       </c>
@@ -5474,7 +5803,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:39">
+    <row r="46" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="B46" t="s">
         <v>0</v>
       </c>
@@ -5590,7 +5922,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:39">
+    <row r="47" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="B47" t="s">
         <v>0</v>
       </c>
@@ -5706,7 +6041,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:39">
+    <row r="48" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="B48" t="s">
         <v>0</v>
       </c>
@@ -5822,7 +6160,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:39">
+    <row r="49" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="B49" t="s">
         <v>1</v>
       </c>
@@ -5938,7 +6279,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:39">
+    <row r="50" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="B50" t="s">
         <v>0</v>
       </c>
@@ -6054,7 +6398,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:39">
+    <row r="51" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="B51" t="s">
         <v>0</v>
       </c>
@@ -6170,7 +6517,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:39">
+    <row r="52" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="B52" t="s">
         <v>0</v>
       </c>
@@ -6286,7 +6636,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:39">
+    <row r="53" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="B53" t="s">
         <v>0</v>
       </c>
@@ -6402,7 +6755,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:39">
+    <row r="54" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="B54" t="s">
         <v>0</v>
       </c>
@@ -6518,7 +6874,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:39">
+    <row r="55" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="B55" t="s">
         <v>0</v>
       </c>
@@ -6634,7 +6993,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:39">
+    <row r="56" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="B56" t="s">
         <v>0</v>
       </c>
@@ -6750,7 +7112,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:39">
+    <row r="57" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="B57" t="s">
         <v>0</v>
       </c>
@@ -6866,7 +7231,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:39">
+    <row r="58" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="B58" t="s">
         <v>0</v>
       </c>
@@ -6982,7 +7350,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="1:39">
+    <row r="59" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="B59" t="s">
         <v>0</v>
       </c>
@@ -7098,7 +7469,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:39">
+    <row r="60" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="B60" t="s">
         <v>0</v>
       </c>
@@ -7214,7 +7588,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:39">
+    <row r="61" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="C61" t="s">
         <v>0</v>
       </c>
@@ -7246,7 +7623,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:39">
+    <row r="62" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="B62" t="s">
         <v>2</v>
       </c>
@@ -7362,7 +7742,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:39">
+    <row r="63" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="B63" t="s">
         <v>0</v>
       </c>
@@ -7478,7 +7861,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:39">
+    <row r="64" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="B64" t="s">
         <v>0</v>
       </c>
@@ -7594,7 +7980,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:39">
+    <row r="65" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="B65" t="s">
         <v>0</v>
       </c>
@@ -7710,7 +8099,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:39">
+    <row r="66" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="B66" t="s">
         <v>1</v>
       </c>
@@ -7826,7 +8218,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:39">
+    <row r="67" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="B67" t="s">
         <v>1</v>
       </c>
@@ -7942,7 +8337,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:39">
+    <row r="68" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="B68" t="s">
         <v>0</v>
       </c>
@@ -8058,7 +8456,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:39">
+    <row r="69" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="B69" t="s">
         <v>0</v>
       </c>
@@ -8174,7 +8575,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:39">
+    <row r="70" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="B70" t="s">
         <v>0</v>
       </c>
@@ -8290,7 +8694,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:39">
+    <row r="71" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="B71" t="s">
         <v>0</v>
       </c>
@@ -8406,7 +8813,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:39">
+    <row r="72" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="B72" t="s">
         <v>0</v>
       </c>
@@ -8522,7 +8932,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:39">
+    <row r="73" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="B73" t="s">
         <v>0</v>
       </c>
@@ -8638,7 +9051,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:39">
+    <row r="74" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="B74" t="s">
         <v>0</v>
       </c>
@@ -8754,7 +9170,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:39">
+    <row r="75" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="B75" t="s">
         <v>0</v>
       </c>
@@ -8870,7 +9289,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:39">
+    <row r="76" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="B76" t="s">
         <v>2</v>
       </c>
@@ -8986,7 +9408,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:39">
+    <row r="77" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="B77" t="s">
         <v>1</v>
       </c>
@@ -9102,7 +9527,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:39">
+    <row r="78" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="B78" t="s">
         <v>0</v>
       </c>
@@ -9218,7 +9646,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:39">
+    <row r="79" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="B79" t="s">
         <v>0</v>
       </c>
@@ -9334,7 +9765,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:39">
+    <row r="80" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="B80" t="s">
         <v>0</v>
       </c>
@@ -9450,7 +9884,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:39">
+    <row r="81" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="B81" t="s">
         <v>0</v>
       </c>
@@ -9566,7 +10003,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:39">
+    <row r="82" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="B82" t="s">
         <v>0</v>
       </c>
@@ -9682,7 +10122,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:39">
+    <row r="83" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="B83" t="s">
         <v>0</v>
       </c>
@@ -9798,7 +10241,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:39">
+    <row r="84" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="B84" t="s">
         <v>0</v>
       </c>
@@ -9914,7 +10360,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:39">
+    <row r="85" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="B85" t="s">
         <v>0</v>
       </c>
@@ -10030,7 +10479,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:39">
+    <row r="86" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="B86" t="s">
         <v>0</v>
       </c>
@@ -10146,7 +10598,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:39">
+    <row r="87" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A87" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="B87" t="s">
         <v>0</v>
       </c>
@@ -10262,7 +10717,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:39">
+    <row r="88" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A88" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="B88" t="s">
         <v>0</v>
       </c>
@@ -10378,7 +10836,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:39">
+    <row r="89" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A89" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="B89" t="s">
         <v>0</v>
       </c>
@@ -10494,7 +10955,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:39">
+    <row r="90" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A90" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="B90" t="s">
         <v>0</v>
       </c>
@@ -10610,7 +11074,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:39">
+    <row r="91" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A91" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="B91" t="s">
         <v>0</v>
       </c>
@@ -10726,7 +11193,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:39">
+    <row r="92" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A92" s="4" t="s">
+        <v>6</v>
+      </c>
       <c r="B92" t="s">
         <v>0</v>
       </c>
@@ -10842,7 +11312,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:39">
+    <row r="93" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A93" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="B93" t="s">
         <v>0</v>
       </c>
@@ -10958,7 +11431,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:39">
+    <row r="94" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A94" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="B94" t="s">
         <v>0</v>
       </c>
@@ -11074,7 +11550,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:39">
+    <row r="95" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A95" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="B95" t="s">
         <v>0</v>
       </c>
@@ -11190,7 +11669,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:39">
+    <row r="96" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A96" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="B96" t="s">
         <v>0</v>
       </c>
@@ -11306,7 +11788,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:39">
+    <row r="97" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A97" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="B97" t="s">
         <v>0</v>
       </c>
@@ -11422,7 +11907,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="98" spans="1:39">
+    <row r="98" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A98" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="B98" t="s">
         <v>1</v>
       </c>
@@ -11538,7 +12026,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="99" spans="1:39">
+    <row r="99" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A99" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="B99" t="s">
         <v>0</v>
       </c>
@@ -11654,7 +12145,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:39">
+    <row r="100" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A100" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="B100" t="s">
         <v>0</v>
       </c>
@@ -11770,7 +12264,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:39">
+    <row r="101" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A101" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="B101" t="s">
         <v>0</v>
       </c>
@@ -11886,7 +12383,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:39">
+    <row r="102" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A102" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="B102" t="s">
         <v>0</v>
       </c>
@@ -12002,7 +12502,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:39">
+    <row r="103" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A103" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="B103" t="s">
         <v>0</v>
       </c>
@@ -12118,7 +12621,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:39">
+    <row r="104" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A104" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="B104" t="s">
         <v>1</v>
       </c>
@@ -12234,7 +12740,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:39">
+    <row r="105" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A105" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="B105" t="s">
         <v>0</v>
       </c>
@@ -12350,7 +12859,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:39">
+    <row r="106" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A106" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="B106" t="s">
         <v>0</v>
       </c>
@@ -12466,7 +12978,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:39">
+    <row r="107" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A107" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="B107" t="s">
         <v>0</v>
       </c>
@@ -12582,7 +13097,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:39">
+    <row r="108" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A108" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="B108" t="s">
         <v>0</v>
       </c>
@@ -12698,7 +13216,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:39">
+    <row r="109" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A109" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="B109" t="s">
         <v>1</v>
       </c>
@@ -12814,7 +13335,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:39">
+    <row r="110" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A110" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="B110" t="s">
         <v>0</v>
       </c>
@@ -12930,7 +13454,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:39">
+    <row r="111" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A111" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="B111" t="s">
         <v>0</v>
       </c>
@@ -13046,7 +13573,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:39">
+    <row r="112" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A112" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="B112" t="s">
         <v>0</v>
       </c>
@@ -13162,7 +13692,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:39">
+    <row r="113" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A113" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="B113" t="s">
         <v>0</v>
       </c>
@@ -13278,7 +13811,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:39">
+    <row r="114" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A114" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="B114" t="s">
         <v>0</v>
       </c>
@@ -13394,7 +13930,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:39">
+    <row r="115" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A115" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="B115" t="s">
         <v>0</v>
       </c>
@@ -13510,7 +14049,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:39">
+    <row r="116" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A116" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="B116" t="s">
         <v>0</v>
       </c>
@@ -13626,7 +14168,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:39">
+    <row r="117" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A117" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="B117" t="s">
         <v>0</v>
       </c>
@@ -13742,7 +14287,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:39">
+    <row r="118" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A118" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="B118" t="s">
         <v>1</v>
       </c>
@@ -13858,7 +14406,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:39">
+    <row r="119" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A119" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="B119" t="s">
         <v>1</v>
       </c>
@@ -13974,7 +14525,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:39">
+    <row r="120" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A120" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="B120" t="s">
         <v>1</v>
       </c>
@@ -14090,7 +14644,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:39">
+    <row r="121" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A121" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="B121" t="s">
         <v>1</v>
       </c>
@@ -14206,7 +14763,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:39">
+    <row r="122" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A122" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="B122" t="s">
         <v>0</v>
       </c>
@@ -14322,7 +14882,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:39">
+    <row r="123" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A123" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="B123" t="s">
         <v>0</v>
       </c>
@@ -14438,7 +15001,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:39">
+    <row r="124" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A124" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="B124" t="s">
         <v>0</v>
       </c>
@@ -14554,7 +15120,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:39">
+    <row r="125" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A125" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="B125" t="s">
         <v>0</v>
       </c>
@@ -14670,7 +15239,10 @@
         <v>3</v>
       </c>
     </row>
-    <row r="126" spans="1:39">
+    <row r="126" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A126" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="B126" t="s">
         <v>0</v>
       </c>
@@ -14786,7 +15358,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:39">
+    <row r="127" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A127" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="B127" t="s">
         <v>0</v>
       </c>
@@ -14902,7 +15477,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:39">
+    <row r="128" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A128" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="B128" t="s">
         <v>0</v>
       </c>
@@ -15018,7 +15596,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:39">
+    <row r="129" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A129" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="B129" t="s">
         <v>0</v>
       </c>
@@ -15134,7 +15715,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:39">
+    <row r="130" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A130" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="B130" t="s">
         <v>0</v>
       </c>
@@ -15250,7 +15834,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:39">
+    <row r="131" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A131" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="B131" t="s">
         <v>0</v>
       </c>
@@ -15366,7 +15953,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:39">
+    <row r="132" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A132" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="B132" t="s">
         <v>0</v>
       </c>
@@ -15482,7 +16072,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:39">
+    <row r="133" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A133" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="B133" t="s">
         <v>0</v>
       </c>
@@ -15598,7 +16191,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:39">
+    <row r="134" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A134" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="B134" t="s">
         <v>0</v>
       </c>
@@ -15714,7 +16310,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:39">
+    <row r="135" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A135" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="B135" t="s">
         <v>0</v>
       </c>
@@ -15830,7 +16429,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:39">
+    <row r="136" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A136" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="B136" t="s">
         <v>0</v>
       </c>
@@ -15946,7 +16548,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:39">
+    <row r="137" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A137" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="B137" t="s">
         <v>0</v>
       </c>
@@ -16062,7 +16667,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:39">
+    <row r="138" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A138" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="B138" t="s">
         <v>0</v>
       </c>
@@ -16178,7 +16786,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:39">
+    <row r="139" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A139" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="B139" t="s">
         <v>0</v>
       </c>
@@ -16294,7 +16905,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:39">
+    <row r="140" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A140" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="B140" t="s">
         <v>0</v>
       </c>
@@ -16410,7 +17024,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:39">
+    <row r="141" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A141" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="B141" t="s">
         <v>0</v>
       </c>
@@ -16526,7 +17143,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:39">
+    <row r="142" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A142" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="B142" t="s">
         <v>0</v>
       </c>
@@ -16642,7 +17262,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:39">
+    <row r="143" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A143" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="B143" t="s">
         <v>0</v>
       </c>
@@ -16758,7 +17381,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:39">
+    <row r="144" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A144" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="B144" t="s">
         <v>0</v>
       </c>
@@ -16874,7 +17500,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="145" spans="1:39">
+    <row r="145" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A145" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="B145" t="s">
         <v>0</v>
       </c>
@@ -16990,7 +17619,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:39">
+    <row r="146" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A146" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="B146" t="s">
         <v>0</v>
       </c>
@@ -17106,7 +17738,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:39">
+    <row r="147" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A147" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="B147" t="s">
         <v>0</v>
       </c>
@@ -17222,7 +17857,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:39">
+    <row r="148" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A148" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="B148" t="s">
         <v>0</v>
       </c>
@@ -17338,7 +17976,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:39">
+    <row r="149" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A149" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="B149" t="s">
         <v>0</v>
       </c>
@@ -17454,7 +18095,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:39">
+    <row r="150" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A150" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="B150" t="s">
         <v>0</v>
       </c>
@@ -17570,7 +18214,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:39">
+    <row r="151" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A151" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="B151" t="s">
         <v>0</v>
       </c>
@@ -17686,7 +18333,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:39">
+    <row r="152" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A152" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="B152" t="s">
         <v>0</v>
       </c>
@@ -17802,7 +18452,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:39">
+    <row r="153" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A153" s="4" t="s">
+        <v>8</v>
+      </c>
       <c r="B153" t="s">
         <v>0</v>
       </c>
@@ -17918,7 +18571,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:39">
+    <row r="154" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A154" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="B154" t="s">
         <v>0</v>
       </c>
@@ -18034,7 +18690,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:39">
+    <row r="155" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A155" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="B155" t="s">
         <v>3</v>
       </c>
@@ -18150,7 +18809,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:39">
+    <row r="156" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A156" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="B156" t="s">
         <v>0</v>
       </c>
@@ -18266,7 +18928,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:39">
+    <row r="157" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A157" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="B157" t="s">
         <v>0</v>
       </c>
@@ -18382,7 +19047,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:39">
+    <row r="158" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A158" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="B158" t="s">
         <v>0</v>
       </c>
@@ -18498,7 +19166,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:39">
+    <row r="159" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A159" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="B159" t="s">
         <v>0</v>
       </c>
@@ -18614,7 +19285,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:39">
+    <row r="160" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A160" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="B160" t="s">
         <v>0</v>
       </c>
@@ -18730,7 +19404,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:39">
+    <row r="161" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A161" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="B161" t="s">
         <v>0</v>
       </c>
@@ -18846,7 +19523,10 @@
         <v>3</v>
       </c>
     </row>
-    <row r="162" spans="1:39">
+    <row r="162" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A162" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="B162" t="s">
         <v>0</v>
       </c>
@@ -18962,7 +19642,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:39">
+    <row r="163" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A163" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="B163" t="s">
         <v>0</v>
       </c>
@@ -19078,7 +19761,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:39">
+    <row r="164" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A164" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="B164" t="s">
         <v>0</v>
       </c>
@@ -19194,7 +19880,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:39">
+    <row r="165" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A165" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="B165" t="s">
         <v>0</v>
       </c>
@@ -19310,7 +19999,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:39">
+    <row r="166" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A166" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="B166" t="s">
         <v>0</v>
       </c>
@@ -19426,7 +20118,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="167" spans="1:39">
+    <row r="167" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A167" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="B167" t="s">
         <v>0</v>
       </c>
@@ -19542,7 +20237,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="168" spans="1:39">
+    <row r="168" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A168" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="B168" t="s">
         <v>0</v>
       </c>
@@ -19658,7 +20356,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:39">
+    <row r="169" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A169" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="B169" t="s">
         <v>0</v>
       </c>
@@ -19774,7 +20475,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:39">
+    <row r="170" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A170" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="B170" t="s">
         <v>0</v>
       </c>
@@ -19890,7 +20594,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:39">
+    <row r="171" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A171" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="B171" t="s">
         <v>0</v>
       </c>
@@ -20006,7 +20713,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:39">
+    <row r="172" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A172" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="B172" t="s">
         <v>0</v>
       </c>
@@ -20122,7 +20832,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="173" spans="1:39">
+    <row r="173" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A173" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="B173" t="s">
         <v>0</v>
       </c>
@@ -20238,7 +20951,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:39">
+    <row r="174" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A174" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="B174" t="s">
         <v>0</v>
       </c>
@@ -20354,7 +21070,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:39">
+    <row r="175" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A175" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="B175" t="s">
         <v>0</v>
       </c>
@@ -20470,7 +21189,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:39">
+    <row r="176" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A176" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="B176" t="s">
         <v>0</v>
       </c>
@@ -20586,7 +21308,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:39">
+    <row r="177" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A177" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="B177" t="s">
         <v>0</v>
       </c>
@@ -20702,7 +21427,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="1:39">
+    <row r="178" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A178" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="B178" t="s">
         <v>0</v>
       </c>
@@ -20818,7 +21546,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:39">
+    <row r="179" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A179" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="B179" t="s">
         <v>0</v>
       </c>
@@ -20934,7 +21665,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:39">
+    <row r="180" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A180" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="B180" t="s">
         <v>0</v>
       </c>
@@ -21050,7 +21784,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:39">
+    <row r="181" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A181" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="B181" t="s">
         <v>0</v>
       </c>
@@ -21166,7 +21903,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="182" spans="1:39">
+    <row r="182" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A182" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="B182" t="s">
         <v>0</v>
       </c>
@@ -21282,7 +22022,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="183" spans="1:39">
+    <row r="183" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A183" s="4" t="s">
+        <v>9</v>
+      </c>
       <c r="B183" t="s">
         <v>0</v>
       </c>
@@ -21398,7 +22141,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:39">
+    <row r="184" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A184" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="B184" t="s">
         <v>0</v>
       </c>
@@ -21514,7 +22260,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:39">
+    <row r="185" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A185" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="B185" t="s">
         <v>0</v>
       </c>
@@ -21630,7 +22379,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="1:39">
+    <row r="186" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A186" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="B186" t="s">
         <v>0</v>
       </c>
@@ -21746,7 +22498,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:39">
+    <row r="187" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A187" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="B187" t="s">
         <v>0</v>
       </c>
@@ -21862,7 +22617,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="1:39">
+    <row r="188" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A188" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="B188" t="s">
         <v>0</v>
       </c>
@@ -21978,7 +22736,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="189" spans="1:39">
+    <row r="189" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A189" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="B189" t="s">
         <v>0</v>
       </c>
@@ -22094,7 +22855,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="190" spans="1:39">
+    <row r="190" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A190" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="B190" t="s">
         <v>0</v>
       </c>
@@ -22210,7 +22974,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="191" spans="1:39">
+    <row r="191" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A191" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="B191" t="s">
         <v>0</v>
       </c>
@@ -22326,7 +23093,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="192" spans="1:39">
+    <row r="192" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A192" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="B192" t="s">
         <v>0</v>
       </c>
@@ -22442,7 +23212,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="193" spans="1:39">
+    <row r="193" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A193" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="B193" t="s">
         <v>0</v>
       </c>
@@ -22558,7 +23331,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="194" spans="1:39">
+    <row r="194" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A194" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="B194" t="s">
         <v>0</v>
       </c>
@@ -22674,7 +23450,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="195" spans="1:39">
+    <row r="195" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A195" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="B195" t="s">
         <v>0</v>
       </c>
@@ -22790,7 +23569,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="196" spans="1:39">
+    <row r="196" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A196" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="B196" t="s">
         <v>0</v>
       </c>
@@ -22906,7 +23688,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="1:39">
+    <row r="197" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A197" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="B197" t="s">
         <v>0</v>
       </c>
@@ -23022,7 +23807,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="198" spans="1:39">
+    <row r="198" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A198" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="B198" t="s">
         <v>0</v>
       </c>
@@ -23138,7 +23926,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="199" spans="1:39">
+    <row r="199" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A199" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="B199" t="s">
         <v>0</v>
       </c>
@@ -23254,7 +24045,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="200" spans="1:39">
+    <row r="200" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A200" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="B200" t="s">
         <v>0</v>
       </c>
@@ -23370,7 +24164,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="201" spans="1:39">
+    <row r="201" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A201" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="B201" t="s">
         <v>0</v>
       </c>
@@ -23486,7 +24283,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="202" spans="1:39">
+    <row r="202" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A202" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="B202" t="s">
         <v>1</v>
       </c>
@@ -23602,7 +24402,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="203" spans="1:39">
+    <row r="203" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A203" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="B203" t="s">
         <v>0</v>
       </c>
@@ -23718,7 +24521,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="204" spans="1:39">
+    <row r="204" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A204" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="B204" t="s">
         <v>0</v>
       </c>
@@ -23834,7 +24640,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="205" spans="1:39">
+    <row r="205" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A205" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="B205" t="s">
         <v>0</v>
       </c>
@@ -23950,7 +24759,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="206" spans="1:39">
+    <row r="206" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A206" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="B206" t="s">
         <v>0</v>
       </c>
@@ -24066,7 +24878,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="207" spans="1:39">
+    <row r="207" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A207" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="B207" t="s">
         <v>0</v>
       </c>
@@ -24182,7 +24997,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="208" spans="1:39">
+    <row r="208" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A208" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="B208" t="s">
         <v>0</v>
       </c>
@@ -24298,7 +25116,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="209" spans="1:39">
+    <row r="209" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A209" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="B209" t="s">
         <v>0</v>
       </c>
@@ -24414,7 +25235,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="210" spans="1:39">
+    <row r="210" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A210" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="B210" t="s">
         <v>0</v>
       </c>
@@ -24530,7 +25354,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="211" spans="1:39">
+    <row r="211" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A211" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="B211" t="s">
         <v>0</v>
       </c>
@@ -24646,7 +25473,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="212" spans="1:39">
+    <row r="212" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A212" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="B212" t="s">
         <v>0</v>
       </c>
@@ -24762,7 +25592,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="213" spans="1:39">
+    <row r="213" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A213" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="B213" t="s">
         <v>0</v>
       </c>
@@ -24878,7 +25711,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="214" spans="1:39">
+    <row r="214" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A214" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="B214" t="s">
         <v>0</v>
       </c>
@@ -24994,7 +25830,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="215" spans="1:39">
+    <row r="215" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A215" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="B215" t="s">
         <v>0</v>
       </c>
@@ -25110,7 +25949,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="216" spans="1:39">
+    <row r="216" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A216" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="B216" t="s">
         <v>0</v>
       </c>
@@ -25226,7 +26068,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="217" spans="1:39">
+    <row r="217" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A217" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="B217" t="s">
         <v>0</v>
       </c>
@@ -25342,7 +26187,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="218" spans="1:39">
+    <row r="218" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A218" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="B218" t="s">
         <v>0</v>
       </c>
@@ -25458,7 +26306,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="219" spans="1:39">
+    <row r="219" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A219" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="B219" t="s">
         <v>0</v>
       </c>
@@ -25574,7 +26425,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="220" spans="1:39">
+    <row r="220" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A220" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="B220" t="s">
         <v>0</v>
       </c>
@@ -25690,7 +26544,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="221" spans="1:39">
+    <row r="221" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A221" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="B221" t="s">
         <v>0</v>
       </c>
@@ -25806,7 +26663,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="222" spans="1:39">
+    <row r="222" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A222" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="B222" t="s">
         <v>0</v>
       </c>
@@ -25922,7 +26782,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="223" spans="1:39">
+    <row r="223" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A223" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="B223" t="s">
         <v>0</v>
       </c>
@@ -26038,7 +26901,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="224" spans="1:39">
+    <row r="224" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A224" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="B224" t="s">
         <v>0</v>
       </c>
@@ -26154,7 +27020,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="225" spans="1:39">
+    <row r="225" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A225" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="B225" t="s">
         <v>0</v>
       </c>
@@ -26270,7 +27139,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="226" spans="1:39">
+    <row r="226" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A226" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="B226" t="s">
         <v>0</v>
       </c>
@@ -26386,7 +27258,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="227" spans="1:39">
+    <row r="227" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A227" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="B227" t="s">
         <v>0</v>
       </c>
@@ -26502,7 +27377,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="228" spans="1:39">
+    <row r="228" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A228" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="B228" t="s">
         <v>0</v>
       </c>
@@ -26618,7 +27496,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="229" spans="1:39">
+    <row r="229" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A229" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="B229" t="s">
         <v>0</v>
       </c>
@@ -26734,7 +27615,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="230" spans="1:39">
+    <row r="230" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A230" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="B230" t="s">
         <v>0</v>
       </c>
@@ -26850,7 +27734,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="231" spans="1:39">
+    <row r="231" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A231" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="B231" t="s">
         <v>0</v>
       </c>
@@ -26966,7 +27853,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="232" spans="1:39">
+    <row r="232" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A232" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="B232" t="s">
         <v>0</v>
       </c>
@@ -27082,7 +27972,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="233" spans="1:39">
+    <row r="233" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A233" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="B233" t="s">
         <v>0</v>
       </c>
@@ -27198,7 +28091,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="234" spans="1:39">
+    <row r="234" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A234" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="B234" t="s">
         <v>0</v>
       </c>
@@ -27314,7 +28210,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="235" spans="1:39">
+    <row r="235" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A235" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="B235" t="s">
         <v>0</v>
       </c>
@@ -27430,7 +28329,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="236" spans="1:39">
+    <row r="236" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A236" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="B236" t="s">
         <v>0</v>
       </c>
@@ -27546,7 +28448,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="237" spans="1:39">
+    <row r="237" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A237" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="B237" t="s">
         <v>0</v>
       </c>
@@ -27662,7 +28567,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="238" spans="1:39">
+    <row r="238" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A238" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="B238" t="s">
         <v>0</v>
       </c>
@@ -27778,7 +28686,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="239" spans="1:39">
+    <row r="239" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A239" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="B239" t="s">
         <v>0</v>
       </c>
@@ -27894,7 +28805,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="240" spans="1:39">
+    <row r="240" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A240" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="B240" t="s">
         <v>0</v>
       </c>
@@ -28010,7 +28924,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="241" spans="1:39">
+    <row r="241" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A241" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="B241" t="s">
         <v>0</v>
       </c>
@@ -28126,7 +29043,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="242" spans="1:39">
+    <row r="242" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A242" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="B242" t="s">
         <v>0</v>
       </c>
@@ -28242,7 +29162,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="243" spans="1:39">
+    <row r="243" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A243" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="B243" t="s">
         <v>0</v>
       </c>
@@ -28358,7 +29281,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="244" spans="1:39">
+    <row r="244" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A244" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="B244" t="s">
         <v>0</v>
       </c>
@@ -28474,7 +29400,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="245" spans="1:39">
+    <row r="245" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A245" s="4" t="s">
+        <v>11</v>
+      </c>
       <c r="B245" t="s">
         <v>0</v>
       </c>
@@ -28590,7 +29519,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="246" spans="1:39">
+    <row r="246" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A246" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="B246" t="s">
         <v>0</v>
       </c>
@@ -28706,7 +29638,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="247" spans="1:39">
+    <row r="247" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A247" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="B247" t="s">
         <v>0</v>
       </c>
@@ -28822,7 +29757,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="248" spans="1:39">
+    <row r="248" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A248" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="B248" t="s">
         <v>0</v>
       </c>
@@ -28938,7 +29876,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="249" spans="1:39">
+    <row r="249" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A249" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="B249" t="s">
         <v>0</v>
       </c>
@@ -29054,7 +29995,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="250" spans="1:39">
+    <row r="250" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A250" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="B250" t="s">
         <v>0</v>
       </c>
@@ -29170,7 +30114,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="251" spans="1:39">
+    <row r="251" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A251" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="B251" t="s">
         <v>0</v>
       </c>
@@ -29286,7 +30233,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="252" spans="1:39">
+    <row r="252" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A252" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="B252" t="s">
         <v>0</v>
       </c>
@@ -29402,7 +30352,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="253" spans="1:39">
+    <row r="253" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A253" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="B253" t="s">
         <v>0</v>
       </c>
@@ -29518,7 +30471,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="254" spans="1:39">
+    <row r="254" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A254" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="B254" t="s">
         <v>0</v>
       </c>
@@ -29634,7 +30590,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="255" spans="1:39">
+    <row r="255" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A255" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="B255" t="s">
         <v>0</v>
       </c>
@@ -29750,7 +30709,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="256" spans="1:39">
+    <row r="256" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A256" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="B256" t="s">
         <v>0</v>
       </c>
@@ -29866,7 +30828,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="257" spans="1:39">
+    <row r="257" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A257" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="B257" t="s">
         <v>0</v>
       </c>
@@ -29982,7 +30947,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="258" spans="1:39">
+    <row r="258" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A258" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="B258" t="s">
         <v>0</v>
       </c>
@@ -30098,7 +31066,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="259" spans="1:39">
+    <row r="259" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A259" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="B259" t="s">
         <v>0</v>
       </c>
@@ -30214,7 +31185,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="260" spans="1:39">
+    <row r="260" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A260" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="B260" t="s">
         <v>0</v>
       </c>
@@ -30330,7 +31304,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="261" spans="1:39">
+    <row r="261" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A261" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="B261" t="s">
         <v>0</v>
       </c>
@@ -30446,7 +31423,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="262" spans="1:39">
+    <row r="262" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A262" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="B262" t="s">
         <v>0</v>
       </c>
@@ -30562,7 +31542,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="263" spans="1:39">
+    <row r="263" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A263" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="B263" t="s">
         <v>0</v>
       </c>
@@ -30678,7 +31661,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="264" spans="1:39">
+    <row r="264" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A264" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="B264" t="s">
         <v>0</v>
       </c>
@@ -30794,7 +31780,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="265" spans="1:39">
+    <row r="265" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A265" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="B265" t="s">
         <v>0</v>
       </c>
@@ -30910,7 +31899,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="266" spans="1:39">
+    <row r="266" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A266" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="B266" t="s">
         <v>0</v>
       </c>
@@ -31026,7 +32018,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="267" spans="1:39">
+    <row r="267" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A267" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="B267" t="s">
         <v>0</v>
       </c>
@@ -31142,7 +32137,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="268" spans="1:39">
+    <row r="268" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A268" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="B268" t="s">
         <v>0</v>
       </c>
@@ -31258,7 +32256,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="269" spans="1:39">
+    <row r="269" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A269" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="B269" t="s">
         <v>0</v>
       </c>
@@ -31374,7 +32375,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="270" spans="1:39">
+    <row r="270" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A270" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="B270" t="s">
         <v>0</v>
       </c>
@@ -31490,7 +32494,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="271" spans="1:39">
+    <row r="271" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A271" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="B271" t="s">
         <v>0</v>
       </c>
@@ -31606,7 +32613,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="272" spans="1:39">
+    <row r="272" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A272" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="B272" t="s">
         <v>0</v>
       </c>
@@ -31722,7 +32732,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="273" spans="1:39">
+    <row r="273" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A273" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="B273" t="s">
         <v>3</v>
       </c>
@@ -31838,7 +32851,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="274" spans="1:39">
+    <row r="274" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A274" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="B274" t="s">
         <v>3</v>
       </c>
@@ -31954,7 +32970,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="275" spans="1:39">
+    <row r="275" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A275" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="B275" t="s">
         <v>0</v>
       </c>
@@ -32070,7 +33089,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="276" spans="1:39">
+    <row r="276" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A276" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="B276" t="s">
         <v>0</v>
       </c>
@@ -32186,7 +33208,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="277" spans="1:39">
+    <row r="277" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A277" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="B277" t="s">
         <v>0</v>
       </c>
@@ -32302,7 +33327,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="278" spans="1:39">
+    <row r="278" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A278" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="B278" t="s">
         <v>0</v>
       </c>
@@ -32418,7 +33446,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="279" spans="1:39">
+    <row r="279" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A279" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="B279" t="s">
         <v>0</v>
       </c>
@@ -32534,7 +33565,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="280" spans="1:39">
+    <row r="280" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A280" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="B280" t="s">
         <v>0</v>
       </c>
@@ -32650,7 +33684,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="281" spans="1:39">
+    <row r="281" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A281" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="B281" t="s">
         <v>0</v>
       </c>
@@ -32766,7 +33803,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="282" spans="1:39">
+    <row r="282" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A282" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="B282" t="s">
         <v>1</v>
       </c>
@@ -32882,7 +33922,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="283" spans="1:39">
+    <row r="283" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A283" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="B283" t="s">
         <v>0</v>
       </c>
@@ -32998,7 +34041,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="284" spans="1:39">
+    <row r="284" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A284" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="B284" t="s">
         <v>0</v>
       </c>
@@ -33114,7 +34160,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="285" spans="1:39">
+    <row r="285" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A285" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="B285" t="s">
         <v>0</v>
       </c>
@@ -33230,7 +34279,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="286" spans="1:39">
+    <row r="286" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A286" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="B286" t="s">
         <v>0</v>
       </c>
@@ -33346,7 +34398,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="287" spans="1:39">
+    <row r="287" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A287" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="B287" t="s">
         <v>0</v>
       </c>
@@ -33462,7 +34517,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="288" spans="1:39">
+    <row r="288" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A288" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="B288" t="s">
         <v>0</v>
       </c>
@@ -33578,7 +34636,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="289" spans="1:39">
+    <row r="289" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A289" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="B289" t="s">
         <v>0</v>
       </c>
@@ -33694,7 +34755,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="290" spans="1:39">
+    <row r="290" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A290" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="B290" t="s">
         <v>0</v>
       </c>
@@ -33810,7 +34874,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="291" spans="1:39">
+    <row r="291" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A291" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="B291" t="s">
         <v>0</v>
       </c>
@@ -33926,7 +34993,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="292" spans="1:39">
+    <row r="292" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A292" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="B292" t="s">
         <v>0</v>
       </c>
@@ -34042,7 +35112,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="293" spans="1:39">
+    <row r="293" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A293" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="B293" t="s">
         <v>0</v>
       </c>
@@ -34158,7 +35231,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="294" spans="1:39">
+    <row r="294" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A294" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="B294" t="s">
         <v>0</v>
       </c>
@@ -34274,7 +35350,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="295" spans="1:39">
+    <row r="295" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A295" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="B295" t="s">
         <v>0</v>
       </c>
@@ -34390,7 +35469,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="296" spans="1:39">
+    <row r="296" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A296" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="B296" t="s">
         <v>0</v>
       </c>
@@ -34506,7 +35588,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="297" spans="1:39">
+    <row r="297" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A297" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="B297" t="s">
         <v>3</v>
       </c>
@@ -34622,7 +35707,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="298" spans="1:39">
+    <row r="298" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A298" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="B298" t="s">
         <v>0</v>
       </c>
@@ -34738,7 +35826,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="299" spans="1:39">
+    <row r="299" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A299" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="B299" t="s">
         <v>0</v>
       </c>
@@ -34854,7 +35945,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="300" spans="1:39">
+    <row r="300" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A300" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="B300" t="s">
         <v>0</v>
       </c>
@@ -34970,7 +36064,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="301" spans="1:39">
+    <row r="301" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A301" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="B301" t="s">
         <v>0</v>
       </c>
@@ -35086,7 +36183,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="302" spans="1:39">
+    <row r="302" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A302" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="B302" t="s">
         <v>0</v>
       </c>
@@ -35202,7 +36302,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="303" spans="1:39">
+    <row r="303" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A303" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="B303" t="s">
         <v>0</v>
       </c>
@@ -35318,7 +36421,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="304" spans="1:39">
+    <row r="304" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A304" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="B304" t="s">
         <v>0</v>
       </c>
@@ -35434,7 +36540,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="305" spans="1:39">
+    <row r="305" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A305" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="B305" t="s">
         <v>0</v>
       </c>
@@ -35550,7 +36659,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="306" spans="1:39">
+    <row r="306" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A306" s="4" t="s">
+        <v>13</v>
+      </c>
       <c r="B306" t="s">
         <v>0</v>
       </c>
@@ -35666,7 +36778,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="307" spans="1:39">
+    <row r="307" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A307" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="B307" t="s">
         <v>0</v>
       </c>
@@ -35782,7 +36897,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="308" spans="1:39">
+    <row r="308" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A308" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="B308" t="s">
         <v>0</v>
       </c>
@@ -35898,7 +37016,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="309" spans="1:39">
+    <row r="309" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A309" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="B309" t="s">
         <v>0</v>
       </c>
@@ -36014,7 +37135,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="310" spans="1:39">
+    <row r="310" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A310" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="B310" t="s">
         <v>0</v>
       </c>
@@ -36130,7 +37254,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="311" spans="1:39">
+    <row r="311" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A311" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="B311" t="s">
         <v>2</v>
       </c>
@@ -36246,7 +37373,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="312" spans="1:39">
+    <row r="312" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A312" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="B312" t="s">
         <v>0</v>
       </c>
@@ -36362,7 +37492,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="313" spans="1:39">
+    <row r="313" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A313" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="B313" t="s">
         <v>0</v>
       </c>
@@ -36478,7 +37611,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="314" spans="1:39">
+    <row r="314" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A314" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="B314" t="s">
         <v>0</v>
       </c>
@@ -36594,7 +37730,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="315" spans="1:39">
+    <row r="315" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A315" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="B315" t="s">
         <v>1</v>
       </c>
@@ -36710,7 +37849,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="316" spans="1:39">
+    <row r="316" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A316" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="B316" t="s">
         <v>1</v>
       </c>
@@ -36826,7 +37968,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="317" spans="1:39">
+    <row r="317" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A317" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="B317" t="s">
         <v>0</v>
       </c>
@@ -36942,7 +38087,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="318" spans="1:39">
+    <row r="318" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A318" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="B318" t="s">
         <v>0</v>
       </c>
@@ -37058,7 +38206,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="319" spans="1:39">
+    <row r="319" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A319" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="B319" t="s">
         <v>2</v>
       </c>
@@ -37174,7 +38325,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="320" spans="1:39">
+    <row r="320" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A320" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="B320" t="s">
         <v>0</v>
       </c>
@@ -37290,7 +38444,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="321" spans="1:39">
+    <row r="321" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A321" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="B321" t="s">
         <v>0</v>
       </c>
@@ -37406,7 +38563,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="322" spans="1:39">
+    <row r="322" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A322" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="B322" t="s">
         <v>0</v>
       </c>
@@ -37522,7 +38682,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="323" spans="1:39">
+    <row r="323" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A323" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="B323" t="s">
         <v>0</v>
       </c>
@@ -37638,7 +38801,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="324" spans="1:39">
+    <row r="324" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A324" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="B324" t="s">
         <v>0</v>
       </c>
@@ -37754,7 +38920,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="325" spans="1:39">
+    <row r="325" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A325" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="B325" t="s">
         <v>0</v>
       </c>
@@ -37870,7 +39039,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="326" spans="1:39">
+    <row r="326" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A326" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="B326" t="s">
         <v>1</v>
       </c>
@@ -37986,7 +39158,10 @@
         <v>3</v>
       </c>
     </row>
-    <row r="327" spans="1:39">
+    <row r="327" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A327" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="B327" t="s">
         <v>1</v>
       </c>
@@ -38102,7 +39277,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="328" spans="1:39">
+    <row r="328" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A328" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="B328" t="s">
         <v>1</v>
       </c>
@@ -38218,7 +39396,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="329" spans="1:39">
+    <row r="329" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A329" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="B329" t="s">
         <v>1</v>
       </c>
@@ -38334,7 +39515,10 @@
         <v>3</v>
       </c>
     </row>
-    <row r="330" spans="1:39">
+    <row r="330" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A330" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="B330" t="s">
         <v>1</v>
       </c>
@@ -38450,7 +39634,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="331" spans="1:39">
+    <row r="331" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A331" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="B331" t="s">
         <v>0</v>
       </c>
@@ -38566,7 +39753,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="332" spans="1:39">
+    <row r="332" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A332" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="B332" t="s">
         <v>0</v>
       </c>
@@ -38682,7 +39872,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="333" spans="1:39">
+    <row r="333" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A333" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="B333" t="s">
         <v>1</v>
       </c>
@@ -38798,7 +39991,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="334" spans="1:39">
+    <row r="334" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A334" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="B334" t="s">
         <v>0</v>
       </c>
@@ -38914,7 +40110,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="335" spans="1:39">
+    <row r="335" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A335" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="B335" t="s">
         <v>0</v>
       </c>
@@ -39030,7 +40229,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="336" spans="1:39">
+    <row r="336" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A336" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="B336" t="s">
         <v>0</v>
       </c>
@@ -39146,7 +40348,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="337" spans="1:39">
+    <row r="337" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A337" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="B337" t="s">
         <v>0</v>
       </c>
@@ -39262,7 +40467,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="338" spans="1:39">
+    <row r="338" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A338" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="B338" t="s">
         <v>0</v>
       </c>
@@ -39378,7 +40586,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="339" spans="1:39">
+    <row r="339" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A339" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="B339" t="s">
         <v>3</v>
       </c>
@@ -39494,7 +40705,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="340" spans="1:39">
+    <row r="340" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A340" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="B340" t="s">
         <v>2</v>
       </c>
@@ -39610,7 +40824,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="341" spans="1:39">
+    <row r="341" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A341" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="B341" t="s">
         <v>0</v>
       </c>
@@ -39726,7 +40943,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="342" spans="1:39">
+    <row r="342" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A342" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="B342" t="s">
         <v>0</v>
       </c>
@@ -39842,7 +41062,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="343" spans="1:39">
+    <row r="343" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A343" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="B343" t="s">
         <v>0</v>
       </c>
@@ -39958,7 +41181,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="344" spans="1:39">
+    <row r="344" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A344" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="B344" t="s">
         <v>0</v>
       </c>
@@ -40074,7 +41300,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="345" spans="1:39">
+    <row r="345" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A345" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="B345" t="s">
         <v>1</v>
       </c>
@@ -40190,7 +41419,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="346" spans="1:39">
+    <row r="346" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A346" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="B346" t="s">
         <v>0</v>
       </c>
@@ -40306,7 +41538,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="347" spans="1:39">
+    <row r="347" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A347" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="B347" t="s">
         <v>1</v>
       </c>
@@ -40422,7 +41657,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="348" spans="1:39">
+    <row r="348" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A348" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="B348" t="s">
         <v>0</v>
       </c>
@@ -40538,7 +41776,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="349" spans="1:39">
+    <row r="349" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A349" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="B349" t="s">
         <v>0</v>
       </c>
@@ -40654,7 +41895,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="350" spans="1:39">
+    <row r="350" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A350" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="B350" t="s">
         <v>0</v>
       </c>
@@ -40770,7 +42014,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="351" spans="1:39">
+    <row r="351" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A351" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="B351" t="s">
         <v>0</v>
       </c>
@@ -40886,7 +42133,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="352" spans="1:39">
+    <row r="352" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A352" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="B352" t="s">
         <v>0</v>
       </c>
@@ -41002,7 +42252,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="353" spans="1:39">
+    <row r="353" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A353" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="B353" t="s">
         <v>0</v>
       </c>
@@ -41118,7 +42371,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="354" spans="1:39">
+    <row r="354" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A354" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="B354" t="s">
         <v>0</v>
       </c>
@@ -41234,7 +42490,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="355" spans="1:39">
+    <row r="355" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A355" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="B355" t="s">
         <v>0</v>
       </c>
@@ -41350,7 +42609,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="356" spans="1:39">
+    <row r="356" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A356" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="B356" t="s">
         <v>0</v>
       </c>
@@ -41466,7 +42728,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="357" spans="1:39">
+    <row r="357" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A357" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="B357" t="s">
         <v>0</v>
       </c>
@@ -41582,7 +42847,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="358" spans="1:39">
+    <row r="358" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A358" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="B358" t="s">
         <v>1</v>
       </c>
@@ -41698,7 +42966,10 @@
         <v>3</v>
       </c>
     </row>
-    <row r="359" spans="1:39">
+    <row r="359" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A359" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="B359" t="s">
         <v>3</v>
       </c>
@@ -41814,7 +43085,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="360" spans="1:39">
+    <row r="360" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A360" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="B360" t="s">
         <v>0</v>
       </c>
@@ -41930,7 +43204,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="361" spans="1:39">
+    <row r="361" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A361" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="B361" t="s">
         <v>0</v>
       </c>
@@ -42046,7 +43323,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="362" spans="1:39">
+    <row r="362" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A362" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="B362" t="s">
         <v>0</v>
       </c>
@@ -42162,7 +43442,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="363" spans="1:39">
+    <row r="363" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A363" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="B363" t="s">
         <v>0</v>
       </c>
@@ -42278,7 +43561,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="364" spans="1:39">
+    <row r="364" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A364" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="B364" t="s">
         <v>0</v>
       </c>
@@ -42394,7 +43680,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="365" spans="1:39">
+    <row r="365" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A365" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="B365" t="s">
         <v>0</v>
       </c>
@@ -42510,7 +43799,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="366" spans="1:39">
+    <row r="366" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A366" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="B366" t="s">
         <v>0</v>
       </c>
@@ -42626,7 +43918,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="367" spans="1:39">
+    <row r="367" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A367" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="B367" t="s">
         <v>0</v>
       </c>
@@ -42743,6 +44038,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>